<commit_message>
Generated gerber files for thruster board, worked on APB BOM
</commit_message>
<xml_diff>
--- a/TAUV- Powerboard_22-23/TAUV-Thruster_Power/Project Outputs for TAUV-Thruster_Board/BOM/TAUV-Thruster_Board BOM.xlsx
+++ b/TAUV- Powerboard_22-23/TAUV-Thruster_Power/Project Outputs for TAUV-Thruster_Board/BOM/TAUV-Thruster_Board BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eca7b06caa2491f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{6E6FDD1C-11AB-4CBB-AA32-444193D2E221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7E1DEF5-92D4-470B-B816-5CC7315F696A}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{6E6FDD1C-11AB-4CBB-AA32-444193D2E221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49BFF00A-D11E-4372-BC63-F477488F67EF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C6BA664D-3557-452E-9887-EBE4CA75E167}"/>
   </bookViews>
@@ -600,10 +600,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,13 +901,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FB31AC-5552-4B92-A82D-393C6F18F282}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
     <col min="3" max="3" width="12.90625" customWidth="1"/>
     <col min="4" max="5" width="12.6328125" customWidth="1"/>
     <col min="6" max="6" width="17.90625" customWidth="1"/>

</xml_diff>